<commit_message>
get daily historial data
</commit_message>
<xml_diff>
--- a/data/README_data_company.xlsx
+++ b/data/README_data_company.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jupyter연습\factors_affecting_stock_price\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3A7491-3E56-4DD3-8B1D-1AE005C1FD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FC27A4-E374-4AF8-8C24-73D26A12E52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5550" yWindow="1905" windowWidth="20025" windowHeight="12030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34455" yWindow="1845" windowWidth="20025" windowHeight="12030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="항목설명" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
   <si>
     <t>개인매수지속일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -383,6 +383,18 @@
   </si>
   <si>
     <t>PrivateEquity_Purchase_number_of_consecutive_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>close_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>종가 변동률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>close_price_change_rate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -708,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1111,13 +1123,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1125,13 +1137,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1139,13 +1151,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1153,12 +1165,26 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
         <v>77</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>47</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change abbreviation in company data
</commit_message>
<xml_diff>
--- a/data/README_data_company.xlsx
+++ b/data/README_data_company.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jupyter연습\factors_affecting_stock_price\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jupyter연습\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FC27A4-E374-4AF8-8C24-73D26A12E52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAFC8324-01B6-45AA-BD72-F4EDF5AF364E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34455" yWindow="1845" windowWidth="20025" windowHeight="12030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35685" yWindow="675" windowWidth="20025" windowHeight="12030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="항목설명" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
   <si>
     <t>개인매수지속일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -136,14 +136,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Personal_Purchase_amount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Personal_Purchase_amount_change_rate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Foreigner_Purchase_amount</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -237,66 +229,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>pp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pp_cr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fp_cr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>itp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>itp_cr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>penp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>penp_cr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pep</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pep_cr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pp_con_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fp_con_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>itp_con_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>penp_con_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pep_con_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>rc1_pcr</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -366,10 +298,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Personal_Purchase_number_of_consecutive_days</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Foreigner_Purchase_number_of_consecutive_days</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -395,6 +323,114 @@
   </si>
   <si>
     <t>close_price_change_rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기관매수액</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기관매수변동률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기관매수지속일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Institutional_Purchase_amount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retail_Purchase_amount (Retail investor, Indivisual investor)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retail_Purchase_amount_change_rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retail_Purchase_number_of_consecutive_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Institutional_Purchase_amount_change_rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Institutional_Purchase_amount_number_of_consecutive_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>retail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>retail_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>retail_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreigner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreigner_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreigner_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>institution</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>institution_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>institution_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>invtrust</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>invtrust_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>invtrust_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pension</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pension_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pension_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>privequity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>privequity_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>privequity_days</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -720,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -755,22 +791,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" t="s">
-        <v>53</v>
-      </c>
       <c r="E1" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F1" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -784,7 +820,7 @@
         <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -792,10 +828,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
@@ -806,16 +842,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -823,16 +859,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -840,10 +876,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
@@ -854,10 +890,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -868,10 +904,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="D8" t="s">
         <v>1</v>
@@ -882,13 +918,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -896,13 +932,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -910,13 +946,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="C11" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -924,13 +960,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -938,13 +974,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -952,13 +988,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -966,13 +1002,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -980,13 +1016,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -994,13 +1030,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="C17" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1008,16 +1044,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" t="s">
-        <v>83</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1025,13 +1058,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1039,152 +1072,197 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="D20" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="E21" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D25" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>41</v>
       </c>
       <c r="D26" t="s">
-        <v>93</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D27" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D28" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" t="s">
         <v>75</v>
-      </c>
-      <c r="C29" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change file name, get investor data from krx
</commit_message>
<xml_diff>
--- a/data/README_data_company.xlsx
+++ b/data/README_data_company.xlsx
@@ -5,27 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jupyter연습\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jupyter연습\factors_affecting_stock_price\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAFC8324-01B6-45AA-BD72-F4EDF5AF364E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E98D774-6851-4783-B0C4-6B4D1BB73A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35685" yWindow="675" windowWidth="20025" windowHeight="12030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30990" yWindow="195" windowWidth="20025" windowHeight="12030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="항목설명" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="161">
   <si>
     <t>개인매수지속일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -431,6 +439,234 @@
   </si>
   <si>
     <t>privequity_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>투자신탁 : 증권사, 자산운용사 등이 고객의 자산을 이용하여 투자, 펀드 등</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금융투자 : 증권사, 자산운용사 등이 회사자산을 이용하여 투자할 경우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사모펀드 : 고객의 자산을 이용하여 투자.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>은행 : 고객의 예금을 운용하여 투자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보험 : 고객의 보험금을 운용하여 투자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연기금 : 각종 연금, 공제회 기금등을 직접 운용하여 투자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>국가 : 우체국, 보험공사, 주택공사등 공공기관</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기타금융 : 상호저축은행 등</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기타외국인 : 국내에 6개월 이상 거주하는 외국인. 주로 개인투자자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개인 : 일반인이 주식을 매매</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기관 : 개인을 제외한 투자자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>외국인 : 주로 외국계 증권사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기타법인 : 투자기관이 아닌 법인이 투자할 경우, 자사주 매입등</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금융투자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금융투자변동률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금융투자지속일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>은행매수액</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>은행매수변동율</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>은행매수지속일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보험매수액</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보험매수변동율</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보험매수지속일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기타금융매수액</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기타금융매수변동률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기타금융매수지속일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기타법인매수액</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기타법인매수변동률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기타법인매수지속일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기타외국인매수액</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기타외국인매수변동율</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기타외국인매수액지속일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>financial_Investment_amount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>financial_Investment_amount_change_rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>financial_Investment_amount_number_of_consecutive_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>financial</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>financial_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>financial_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bank_amount_change_rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bank_amount_number_of_consecutive_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bank</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bank_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bank_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insurance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bank_amount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insurance_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insurance_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insurance_amount_change_rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insurance_amount_number_of_consecutive_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>financeetc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>financeetc_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>financeetc_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>corporateetc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>corporateetc_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>corporateetc_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreigneretc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreigneretc_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreigneretc_days</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -438,7 +674,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,6 +684,29 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -474,8 +733,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -756,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -898,6 +1161,9 @@
       <c r="D7" t="s">
         <v>5</v>
       </c>
+      <c r="F7" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -912,6 +1178,9 @@
       <c r="D8" t="s">
         <v>1</v>
       </c>
+      <c r="F8" s="3" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -926,6 +1195,9 @@
       <c r="D9" t="s">
         <v>77</v>
       </c>
+      <c r="F9" s="3" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -940,6 +1212,9 @@
       <c r="D10" t="s">
         <v>78</v>
       </c>
+      <c r="F10" s="3" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -954,19 +1229,25 @@
       <c r="D11" t="s">
         <v>79</v>
       </c>
+      <c r="F11" s="3" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
+        <v>135</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -974,13 +1255,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>139</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
+        <v>136</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -988,13 +1272,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>140</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
+        <v>137</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1002,13 +1289,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1016,253 +1306,490 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>103</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C23" t="s">
         <v>73</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" t="s">
+        <v>147</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>144</v>
+      </c>
+      <c r="C25" t="s">
+        <v>141</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>145</v>
+      </c>
+      <c r="C26" t="s">
+        <v>142</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" t="s">
+        <v>146</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>148</v>
+      </c>
+      <c r="C28" t="s">
+        <v>150</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>149</v>
+      </c>
+      <c r="C29" t="s">
+        <v>151</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>152</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>153</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>154</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>155</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>156</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>158</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>159</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>160</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" t="s">
+        <v>41</v>
+      </c>
+      <c r="D44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45" t="s">
         <v>17</v>
       </c>
-      <c r="B21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>18</v>
-      </c>
-      <c r="B22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46" t="s">
         <v>19</v>
       </c>
-      <c r="B23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>20</v>
-      </c>
-      <c r="B24" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" t="s">
+        <v>76</v>
+      </c>
+      <c r="D47" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" t="s">
+        <v>42</v>
+      </c>
+      <c r="D48" t="s">
         <v>21</v>
       </c>
-      <c r="B25" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" t="s">
+        <v>43</v>
+      </c>
+      <c r="D49" t="s">
         <v>22</v>
       </c>
-      <c r="B26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>23</v>
-      </c>
-      <c r="B27" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>24</v>
-      </c>
-      <c r="B28" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>25</v>
-      </c>
-      <c r="B29" t="s">
-        <v>74</v>
-      </c>
-      <c r="C29" t="s">
-        <v>76</v>
-      </c>
-      <c r="D29" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>26</v>
-      </c>
-      <c r="B30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>27</v>
-      </c>
-      <c r="B31" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" t="s">
-        <v>43</v>
-      </c>
-      <c r="D31" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>28</v>
-      </c>
-      <c r="B32" t="s">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
         <v>58</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C50" t="s">
         <v>47</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D50" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>29</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
         <v>60</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C51" t="s">
         <v>45</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D51" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>